<commit_message>
Extra support for temp dirs for optimize tests
</commit_message>
<xml_diff>
--- a/Testing/data/optimize/sphere/optimize.xlsx
+++ b/Testing/data/optimize/sphere/optimize.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Testing/data/optimize/sphere/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF750E4A-99D9-2141-9991-BF38D99D4CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -16,12 +22,12 @@
     <sheet name="deepssm" sheetId="7" r:id="rId7"/>
     <sheet name="landmarks" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -255,12 +261,6 @@
   </si>
   <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>domain_type</t>
-  </si>
-  <si>
-    <t>segmentation</t>
   </si>
   <si>
     <t>ending_regularization</t>
@@ -477,8 +477,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,6 +515,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -780,14 +788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -839,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -865,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -891,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -923,11 +931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C36"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -938,7 +949,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -946,7 +957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -954,7 +965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -962,7 +973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -970,7 +981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -978,7 +989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -986,7 +997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1002,7 +1013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1010,7 +1021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1018,7 +1029,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1026,7 +1037,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1034,7 +1045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1042,7 +1053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1050,7 +1061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1058,7 +1069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1066,7 +1077,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1074,7 +1085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1082,7 +1093,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1090,7 +1101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1098,7 +1109,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1106,7 +1117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1114,7 +1125,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1122,7 +1133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1130,7 +1141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1138,7 +1149,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1146,7 +1157,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1154,7 +1165,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1170,7 +1181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1178,7 +1189,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1186,7 +1197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1194,7 +1205,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1202,7 +1213,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1210,7 +1221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1219,15 +1230,21 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1235,7 +1252,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1243,7 +1260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1251,7 +1268,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -1259,39 +1276,39 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>85</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -1299,136 +1316,132 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
       <c r="B10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>92</v>
       </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>95</v>
       </c>
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>97</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>98</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>100</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>101</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>102</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>103</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>105</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>106</v>
       </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>107</v>
-      </c>
       <c r="B23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1436,56 +1449,60 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>109</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>111</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>113</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1493,24 +1510,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1518,40 +1539,44 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>120</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>125</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B14"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1559,136 +1584,141 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>128</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>132</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>134</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>136</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>137</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>139</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>140</v>
       </c>
-      <c r="B11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>141</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>144</v>
-      </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" t="s">
-        <v>148</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>